<commit_message>
Cambios en la forma de mostrar los productos
</commit_message>
<xml_diff>
--- a/resultados/excels/wallapop/busquedas_wallapop.xlsx
+++ b/resultados/excels/wallapop/busquedas_wallapop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="126">
   <si>
     <t>Fecha</t>
   </si>
@@ -31,166 +31,367 @@
     <t>URL Producto</t>
   </si>
   <si>
-    <t>2025-06-08</t>
-  </si>
-  <si>
-    <t>Lote de lámparas multicolores de Pokémon</t>
-  </si>
-  <si>
-    <t>Cajas Vacías Pokémon - Lote</t>
-  </si>
-  <si>
-    <t>Pokemon Edición Cristal - Game Boy</t>
-  </si>
-  <si>
-    <t>Pokémon Espada - Nintendo Switch</t>
-  </si>
-  <si>
-    <t>Pokedex de Pokémon</t>
-  </si>
-  <si>
-    <t>¡Pokémon ¡A por ti! Pikachu! Switch</t>
-  </si>
-  <si>
-    <t>Pokémon Escudo Nintendo Switch</t>
-  </si>
-  <si>
-    <t>Pokémon Cristal - Game Boy</t>
-  </si>
-  <si>
-    <t>Lote de cartas Pokémon</t>
-  </si>
-  <si>
-    <t>Pokémon Colosseum - GameCube PAL +Memory Card</t>
-  </si>
-  <si>
-    <t>Pokemon Amarillo Game Boy</t>
-  </si>
-  <si>
-    <t>Pokémon Blanco 2 (Alemán).</t>
-  </si>
-  <si>
-    <t>Peluche Celebi Pokémon</t>
-  </si>
-  <si>
-    <t>Pokémon Perla Reluciente Nintendo Switch</t>
-  </si>
-  <si>
-    <t>Pokemon Rojo - Nintendo Game Boy</t>
-  </si>
-  <si>
-    <t>15 €</t>
-  </si>
-  <si>
-    <t>50 €</t>
+    <t>2025-06-10</t>
+  </si>
+  <si>
+    <t>iPhone 13 mini rojo - 128GB</t>
+  </si>
+  <si>
+    <t>iPhone 13 Pro Gris Espacial</t>
+  </si>
+  <si>
+    <t>iPhone 14 negro</t>
+  </si>
+  <si>
+    <t>iPhone 14 Pro - Negro espacial</t>
+  </si>
+  <si>
+    <t>iPhone 15 128GB Azul</t>
+  </si>
+  <si>
+    <t>iPhone 13 256gb helth 100%</t>
+  </si>
+  <si>
+    <t>iPhone 13 blanco 128GB Starlight</t>
+  </si>
+  <si>
+    <t>iPhone 12 Pro Max 256GB Silver</t>
+  </si>
+  <si>
+    <t>iPhone 13 negro 128gb helth 87%</t>
+  </si>
+  <si>
+    <t>iPhone 8 Plus</t>
+  </si>
+  <si>
+    <t>iPhone 13 Pro Max 256 gigas</t>
+  </si>
+  <si>
+    <t>(BCN) iPhone 14 Impecable</t>
+  </si>
+  <si>
+    <t>iPhone 12 Verde 128GB</t>
+  </si>
+  <si>
+    <t>iPhone 13 Azul - Como Nuevo</t>
+  </si>
+  <si>
+    <t>iPhone 12 Pro Max 128GB - Gris Espacial</t>
+  </si>
+  <si>
+    <t>Paquete de Pokémon Evoluciones Prismáticas sellado</t>
+  </si>
+  <si>
+    <t>Pokémon</t>
+  </si>
+  <si>
+    <t>Pokémon HeartGold Oro - Nintendo DS</t>
+  </si>
+  <si>
+    <t>Lote de Cartas Pokémon Antiguas</t>
+  </si>
+  <si>
+    <t>Carta Pokémon Pikachu Vuelo</t>
+  </si>
+  <si>
+    <t>Pokémon Escudo</t>
+  </si>
+  <si>
+    <t>Aventuras Pokémon Juntas ETB selladas</t>
+  </si>
+  <si>
+    <t>Pokémon Negro - Game Boy</t>
+  </si>
+  <si>
+    <t>Cartas Pokémon Vintage - 30 Fossil</t>
+  </si>
+  <si>
+    <t>Cartas Pokémon Vintage - Aquapolis (10)</t>
+  </si>
+  <si>
+    <t>POKEMON SCUDO Switch Juego Multilingüe</t>
+  </si>
+  <si>
+    <t>Paquete de Pokémon Relámpagos Centelleantes – Sellado</t>
+  </si>
+  <si>
+    <t>Pokémon Escudo - Nintendo Switch</t>
+  </si>
+  <si>
+    <t>Pokémon Violeta Nintendo Switch Juego Original</t>
+  </si>
+  <si>
+    <t>Pokémon Ultraluna - Nintendo 3ds - Completo Italia</t>
+  </si>
+  <si>
+    <t>299 €</t>
+  </si>
+  <si>
+    <t>420 €</t>
+  </si>
+  <si>
+    <t>Precio no disponible</t>
+  </si>
+  <si>
+    <t>549 €</t>
+  </si>
+  <si>
+    <t>600 €</t>
+  </si>
+  <si>
+    <t>399 €</t>
+  </si>
+  <si>
+    <t>369 €</t>
+  </si>
+  <si>
+    <t>449 €</t>
+  </si>
+  <si>
+    <t>349 €</t>
+  </si>
+  <si>
+    <t>90 €</t>
+  </si>
+  <si>
+    <t>479 €</t>
+  </si>
+  <si>
+    <t>385 €</t>
+  </si>
+  <si>
+    <t>270 €</t>
+  </si>
+  <si>
+    <t>350 €</t>
+  </si>
+  <si>
+    <t>300 €</t>
+  </si>
+  <si>
+    <t>60 €</t>
+  </si>
+  <si>
+    <t>32 €</t>
+  </si>
+  <si>
+    <t>118 €</t>
+  </si>
+  <si>
+    <t>18 €</t>
+  </si>
+  <si>
+    <t>26,57 €</t>
+  </si>
+  <si>
+    <t>29 €</t>
+  </si>
+  <si>
+    <t>65 €</t>
+  </si>
+  <si>
+    <t>25,50 €</t>
+  </si>
+  <si>
+    <t>14 €</t>
+  </si>
+  <si>
+    <t>5 €</t>
+  </si>
+  <si>
+    <t>28,50 €</t>
+  </si>
+  <si>
+    <t>54,90 €</t>
   </si>
   <si>
     <t>30 €</t>
   </si>
   <si>
-    <t>40 €</t>
-  </si>
-  <si>
-    <t>32 €</t>
-  </si>
-  <si>
-    <t>60 €</t>
-  </si>
-  <si>
-    <t>18 €</t>
-  </si>
-  <si>
-    <t>34 €</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/32/__/c10420p1140602748/i5711319338.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/36/__/c10420p1140607929/i5711351153.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/2v/__/c10420p1140592970/i5711259363.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iu/yw/__/c10420p1140408646/i5710091868.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/0i/__/c10420p1140483808/i5710601526.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/1z/__/c10420p1140551817/i5711004026.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/3k/__/c10420p1140625511/i5711464481.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/0d/__/c10420p1140476910/i5710559416.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/3k/__/c10420p1140625745/i5711465837.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/24/__/c10420p1140558601/i5711044456.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/2u/__/c10420p1140592659/i5711257559.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/15/__/c10420p1140513558/i5710774598.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/3o/__/c10420p1140631285/i5711500434.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/2h/__/c10420p1140574732/i5711144460.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://cdn.wallapop.com/images/10420/iv/1d/__/c10420p1140522778/i5710828187.jpg?pictureSize=W640</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/lotto-lampade-multicolore-pokemon-1140602748</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/cajas-vacias-pokemon-lote-1140607929</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-edicion-cristal-game-boy-1140592970</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-spada-nintendo-switch-1140408646</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokedex-de-pokemon-1140483808</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-let-s-go-pikachu-switch-1140551817</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-escudo-nintendo-switch-1140625511</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-cristal-game-boy-1140476910</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/lote-de-cartas-pokemon-1140625745</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-colosseum-gamecube-pal--memory-card-1140558601</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-amarillo-game-boy-1140592659</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-blanco-2-aleman-1140513558</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/peluche-celebi-pokemon-1140631285</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-perla-reluciente-nintendo-switch-1140574732</t>
-  </si>
-  <si>
-    <t>https://es.wallapop.com/item/pokemon-rojo-nintendo-game-boy-1140522778</t>
+    <t>38 €</t>
+  </si>
+  <si>
+    <t>35 €</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/eo/__/c10420p1141143628/i5715626532.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/dg/__/c10420p1141087578/i5715221282.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/it/7b/__/c10420p1137441282/i5684796059.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/e0/__/c10420p1141113585/i5715402652.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/ed/__/c10420p1141130335/i5715503993.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/eo/__/c10420p1141144367/i5715633636.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/eq/__/c10420p1141146676/i5715649250.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/ei/__/c10420p1141137007/i5715566588.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/ep/__/c10420p1141145004/i5715638033.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/de/__/c10420p1141083953/i5715183476.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/d6/__/c10420p1141073577/i5715078035.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/ez/__/c10420p1141158316/i5715730001.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/en/__/c10420p1141143153/i5715623206.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/c7/__/c10420p1141029009/i5714765892.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/ed/__/c10420p1141130537/i5715505327.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/eq/__/c10420p1141147263/i5715653003.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/0v/__/c10420p1140500614/i5710693036.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/8n/__/c10420p1140863356/i5713628328.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/bd/__/c10420p1140989689/i5714489737.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/f1/__/c10420p1141160645/i5715745717.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/an/__/c10420p1140956432/i5714256788.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/eo/__/c10420p1141144129/i5715631800.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/76/__/c10420p1140794164/i5712989455.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/2q/__/c10420p1140587122/i5711222786.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/er/__/c10420p1141147805/i5715657637.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/dy/__/c10420p1141110300/i5715378304.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/ci/__/c10420p1141042806/i5714853290.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/bp/__/c10420p1141004894/i5714599893.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/ca/__/c10420p1141032281/i5714786774.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://cdn.wallapop.com/images/10420/iv/dw/__/c10420p1141107518/i5715359681.jpg?pictureSize=W640</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-13-mini-rojo-128gb-1141143628</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-13-pro-gris-espacial-1141087578</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-14-negro-1137441282</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-14-pro-negro-espacial-1141113585</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-15-128gb-azul-1141130335</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-13-256gb-negro-1141144367</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-13-blanco-128gb-starlight-1141146676</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-12-pro-max-256gb-silver-1141137007</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-13-negro-128gb-1141145004</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-8-plus-1141083953</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-13-pro-max-256-gigas-1141073577</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/bcn-iphone-14-impecable-1141158316</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-12-verde-128gb-1141143153</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-13-azul-como-nuevo-1141029009</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/iphone-12-pro-max-128gb-gris-espacial-1141130537</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/bundle-pokemon-evoluzioni-prismatiche-sealed-1141147263</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-1140500614</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-heartgold-oro-nintendo-ds-1140863356</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/lotto-carte-pokemon-old-dal-2010-al-2017-1140989689</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/carta-pokemon-pikachu-vuelo-1141160645</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-scudo-1140956432</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-avventure-insieme-etb-sealed-1141144129</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-black-game-boy-1140794164</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/carte-pokemon-vintage-30-fossil-1140587122</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/carte-pokemon-vintage-aquapolis-10-1141147805</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-scudo-switch-gioco-multilingua-1141110300</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-bundle-scintille-folgoranti-sigillato-1141042806</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-scudo-nintendo-switch-1141004894</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-violetto-nintendo-switch-originale-gioco-1141032281</t>
+  </si>
+  <si>
+    <t>https://es.wallapop.com/item/pokemon-ultraluna-nintendo-3ds-completo-italia-1141107518</t>
   </si>
 </sst>
 </file>
@@ -561,7 +762,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -592,13 +793,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -609,13 +810,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -626,13 +827,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -643,13 +844,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -660,13 +861,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -677,13 +878,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -694,13 +895,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -711,13 +912,13 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -728,13 +929,13 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -745,13 +946,13 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -762,13 +963,13 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -779,13 +980,13 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -796,13 +997,13 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -813,13 +1014,13 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -830,13 +1031,778 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
         <v>58</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -871,6 +1837,96 @@
     <hyperlink ref="E15" r:id="rId28"/>
     <hyperlink ref="D16" r:id="rId29"/>
     <hyperlink ref="E16" r:id="rId30"/>
+    <hyperlink ref="D17" r:id="rId31"/>
+    <hyperlink ref="E17" r:id="rId32"/>
+    <hyperlink ref="D18" r:id="rId33"/>
+    <hyperlink ref="E18" r:id="rId34"/>
+    <hyperlink ref="D19" r:id="rId35"/>
+    <hyperlink ref="E19" r:id="rId36"/>
+    <hyperlink ref="D20" r:id="rId37"/>
+    <hyperlink ref="E20" r:id="rId38"/>
+    <hyperlink ref="D21" r:id="rId39"/>
+    <hyperlink ref="E21" r:id="rId40"/>
+    <hyperlink ref="D22" r:id="rId41"/>
+    <hyperlink ref="E22" r:id="rId42"/>
+    <hyperlink ref="D23" r:id="rId43"/>
+    <hyperlink ref="E23" r:id="rId44"/>
+    <hyperlink ref="D24" r:id="rId45"/>
+    <hyperlink ref="E24" r:id="rId46"/>
+    <hyperlink ref="D25" r:id="rId47"/>
+    <hyperlink ref="E25" r:id="rId48"/>
+    <hyperlink ref="D26" r:id="rId49"/>
+    <hyperlink ref="E26" r:id="rId50"/>
+    <hyperlink ref="D27" r:id="rId51"/>
+    <hyperlink ref="E27" r:id="rId52"/>
+    <hyperlink ref="D28" r:id="rId53"/>
+    <hyperlink ref="E28" r:id="rId54"/>
+    <hyperlink ref="D29" r:id="rId55"/>
+    <hyperlink ref="E29" r:id="rId56"/>
+    <hyperlink ref="D30" r:id="rId57"/>
+    <hyperlink ref="E30" r:id="rId58"/>
+    <hyperlink ref="D31" r:id="rId59"/>
+    <hyperlink ref="E31" r:id="rId60"/>
+    <hyperlink ref="D32" r:id="rId61"/>
+    <hyperlink ref="E32" r:id="rId62"/>
+    <hyperlink ref="D33" r:id="rId63"/>
+    <hyperlink ref="E33" r:id="rId64"/>
+    <hyperlink ref="D34" r:id="rId65"/>
+    <hyperlink ref="E34" r:id="rId66"/>
+    <hyperlink ref="D35" r:id="rId67"/>
+    <hyperlink ref="E35" r:id="rId68"/>
+    <hyperlink ref="D36" r:id="rId69"/>
+    <hyperlink ref="E36" r:id="rId70"/>
+    <hyperlink ref="D37" r:id="rId71"/>
+    <hyperlink ref="E37" r:id="rId72"/>
+    <hyperlink ref="D38" r:id="rId73"/>
+    <hyperlink ref="E38" r:id="rId74"/>
+    <hyperlink ref="D39" r:id="rId75"/>
+    <hyperlink ref="E39" r:id="rId76"/>
+    <hyperlink ref="D40" r:id="rId77"/>
+    <hyperlink ref="E40" r:id="rId78"/>
+    <hyperlink ref="D41" r:id="rId79"/>
+    <hyperlink ref="E41" r:id="rId80"/>
+    <hyperlink ref="D42" r:id="rId81"/>
+    <hyperlink ref="E42" r:id="rId82"/>
+    <hyperlink ref="D43" r:id="rId83"/>
+    <hyperlink ref="E43" r:id="rId84"/>
+    <hyperlink ref="D44" r:id="rId85"/>
+    <hyperlink ref="E44" r:id="rId86"/>
+    <hyperlink ref="D45" r:id="rId87"/>
+    <hyperlink ref="E45" r:id="rId88"/>
+    <hyperlink ref="D46" r:id="rId89"/>
+    <hyperlink ref="E46" r:id="rId90"/>
+    <hyperlink ref="D47" r:id="rId91"/>
+    <hyperlink ref="E47" r:id="rId92"/>
+    <hyperlink ref="D48" r:id="rId93"/>
+    <hyperlink ref="E48" r:id="rId94"/>
+    <hyperlink ref="D49" r:id="rId95"/>
+    <hyperlink ref="E49" r:id="rId96"/>
+    <hyperlink ref="D50" r:id="rId97"/>
+    <hyperlink ref="E50" r:id="rId98"/>
+    <hyperlink ref="D51" r:id="rId99"/>
+    <hyperlink ref="E51" r:id="rId100"/>
+    <hyperlink ref="D52" r:id="rId101"/>
+    <hyperlink ref="E52" r:id="rId102"/>
+    <hyperlink ref="D53" r:id="rId103"/>
+    <hyperlink ref="E53" r:id="rId104"/>
+    <hyperlink ref="D54" r:id="rId105"/>
+    <hyperlink ref="E54" r:id="rId106"/>
+    <hyperlink ref="D55" r:id="rId107"/>
+    <hyperlink ref="E55" r:id="rId108"/>
+    <hyperlink ref="D56" r:id="rId109"/>
+    <hyperlink ref="E56" r:id="rId110"/>
+    <hyperlink ref="D57" r:id="rId111"/>
+    <hyperlink ref="E57" r:id="rId112"/>
+    <hyperlink ref="D58" r:id="rId113"/>
+    <hyperlink ref="E58" r:id="rId114"/>
+    <hyperlink ref="D59" r:id="rId115"/>
+    <hyperlink ref="E59" r:id="rId116"/>
+    <hyperlink ref="D60" r:id="rId117"/>
+    <hyperlink ref="E60" r:id="rId118"/>
+    <hyperlink ref="D61" r:id="rId119"/>
+    <hyperlink ref="E61" r:id="rId120"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>